<commit_message>
IF-123 aligned integrations with details
</commit_message>
<xml_diff>
--- a/Integration List.xlsx
+++ b/Integration List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Integration_Hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45432BCF-DC09-4D0E-96BA-3A975BA63198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1475BF8D-7912-4215-9A3E-3D75DEADA351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{199BEFDA-6D70-4001-AC3C-82D1565D7EFD}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="950">
   <si>
     <t>Integration Name</t>
   </si>
@@ -2867,6 +2867,9 @@
   </si>
   <si>
     <t>https://documents.bmc.com/supportu/9.0.22/en-US/Documentation/AWS_Step_Functions.htm</t>
+  </si>
+  <si>
+    <t>https://documents.bmc.com/supportu/9.0.22/en-US/Documentation/Integrations_Main.htm</t>
   </si>
 </sst>
 </file>
@@ -3478,7 +3481,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E8FA005-27E5-472A-A051-61AF55866230}" name="Table1" displayName="Table1" ref="A1:N1048575" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:N1048575" xr:uid="{4E8FA005-27E5-472A-A051-61AF55866230}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N153">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N224">
     <sortCondition ref="A1:A1048575"/>
   </sortState>
   <tableColumns count="14">
@@ -3491,11 +3494,11 @@
     <tableColumn id="12" xr3:uid="{72E937D1-1E81-48AF-9D5B-5296FD29085D}" name="Popularity" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{D93936C9-0BF2-4880-AC31-E950E3533A2A}" name="Provision Integration Linux" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{85AF1488-40E5-4028-A90A-1DEBE758E866}" name="Provision Integration Windows" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{71BAAA46-203B-4F13-88C2-8B0A20CCD608}" name="Service Website" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{68BE37D1-24AA-4951-B61B-A66DE0F8E323}" name="API Documentation" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{7A555FD3-436A-44A0-995F-B8AE4C683CFB}" name="Github Repository" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{04342CFE-80D7-4551-A592-DBC1B2EC691E}" name="Control-M Documentation" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{6F826D3E-8B6A-44DC-B7BD-BAD899C41737}" name="Remove Integration" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{71BAAA46-203B-4F13-88C2-8B0A20CCD608}" name="Service Website" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{68BE37D1-24AA-4951-B61B-A66DE0F8E323}" name="API Documentation" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{7A555FD3-436A-44A0-995F-B8AE4C683CFB}" name="Github Repository" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{04342CFE-80D7-4551-A592-DBC1B2EC691E}" name="Control-M Documentation" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{6F826D3E-8B6A-44DC-B7BD-BAD899C41737}" name="Remove Integration" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3820,8 +3823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EF2D89-2A74-4C7B-886D-75907E86C7AA}">
   <dimension ref="A1:N224"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="M70" sqref="M70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3836,7 +3839,7 @@
     <col min="10" max="10" width="12.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="39.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41" style="1" customWidth="1"/>
     <col min="14" max="14" width="24.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="41.28515625" customWidth="1"/>
     <col min="16" max="16" width="31.7109375" customWidth="1"/>
@@ -7538,7 +7541,7 @@
         <v>328</v>
       </c>
       <c r="B85" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>482</v>
@@ -7582,7 +7585,7 @@
         <v>332</v>
       </c>
       <c r="B86" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>490</v>
@@ -7670,7 +7673,7 @@
         <v>340</v>
       </c>
       <c r="B88" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>481</v>
@@ -7802,7 +7805,7 @@
         <v>352</v>
       </c>
       <c r="B91" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>476</v>
@@ -8109,6 +8112,9 @@
       <c r="A98" s="1" t="s">
         <v>380</v>
       </c>
+      <c r="B98" t="s">
+        <v>566</v>
+      </c>
       <c r="C98" s="1" t="s">
         <v>491</v>
       </c>
@@ -8139,7 +8145,9 @@
       <c r="L98" s="3" t="s">
         <v>836</v>
       </c>
-      <c r="M98"/>
+      <c r="M98" t="s">
+        <v>949</v>
+      </c>
       <c r="N98" s="1" t="s">
         <v>383</v>
       </c>

</xml_diff>

<commit_message>
IF-123: Update Airflow API documentation link
</commit_message>
<xml_diff>
--- a/Integration List.xlsx
+++ b/Integration List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Integration_Hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E15BDA-E7C6-434E-BB0B-41A2BD611AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D136DE5-2496-4419-ACB1-3ACFFC82B623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{199BEFDA-6D70-4001-AC3C-82D1565D7EFD}"/>
   </bookViews>
@@ -2035,15 +2035,9 @@
     <t>https://docs.ansible.com/ansible/latest/collections/ansible/awx/</t>
   </si>
   <si>
-    <t>https://airflow.apache.org/docs/apache-airflow/stable/rest-api-ref.html</t>
-  </si>
-  <si>
     <t>https://nifi.apache.org/docs/nifi-docs/rest-api/index.html</t>
   </si>
   <si>
-    <t>https://docs.astronomer.io/astro/api</t>
-  </si>
-  <si>
     <t>https://docs.automationanywhere.com/bundle/enterprise-v2019/page/api-reference.html</t>
   </si>
   <si>
@@ -2870,6 +2864,12 @@
   </si>
   <si>
     <t>https://documents.bmc.com/supportu/9.0.22/en-US/Documentation/Integrations_Main.htm</t>
+  </si>
+  <si>
+    <t>https://airflow.apache.org/docs/apache-airflow/stable/stable-rest-api-ref.html</t>
+  </si>
+  <si>
+    <t>https://www.astronomer.io/docs/api/</t>
   </si>
 </sst>
 </file>
@@ -3359,7 +3359,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3371,16 +3371,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3834,7 +3830,7 @@
   <dimension ref="A1:N224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H2" sqref="A2:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3903,314 +3899,314 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>563</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>508</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>521</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="2">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>582</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>671</v>
+        <v>948</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>921</v>
-      </c>
-      <c r="N2" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>563</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>506</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="2">
         <v>3</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>584</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>673</v>
+        <v>949</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>923</v>
-      </c>
-      <c r="N3" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>563</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>508</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>521</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="2">
         <v>3</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="2" t="s">
         <v>96</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>603</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>942</v>
-      </c>
-      <c r="N4" s="5" t="s">
+        <v>940</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>512</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>538</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="2">
         <v>4</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="2" t="s">
         <v>119</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>609</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>948</v>
-      </c>
-      <c r="N5" s="5" t="s">
+        <v>946</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>567</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>508</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="2">
         <v>4</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="2" t="s">
         <v>155</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>618</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>909</v>
-      </c>
-      <c r="N6" s="5" t="s">
+        <v>907</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>217</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>563</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>508</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>552</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="2">
         <v>4</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="2" t="s">
         <v>219</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>633</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>888</v>
-      </c>
-      <c r="N7" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>253</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="2" t="s">
         <v>509</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="2">
         <v>3</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="2" t="s">
         <v>254</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>642</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>897</v>
-      </c>
-      <c r="N8" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -4242,13 +4238,13 @@
         <v>589</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>41</v>
@@ -4286,13 +4282,13 @@
         <v>610</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>124</v>
@@ -4330,13 +4326,13 @@
         <v>658</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>331</v>
@@ -4374,13 +4370,13 @@
         <v>665</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>367</v>
@@ -4418,13 +4414,13 @@
         <v>666</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>371</v>
@@ -4462,13 +4458,13 @@
         <v>604</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>100</v>
@@ -4506,13 +4502,13 @@
         <v>649</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>287</v>
@@ -4550,13 +4546,13 @@
         <v>649</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>319</v>
@@ -4594,13 +4590,13 @@
         <v>656</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>323</v>
@@ -4638,13 +4634,13 @@
         <v>661</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>347</v>
@@ -4685,10 +4681,10 @@
         <v>670</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>492</v>
@@ -4726,13 +4722,13 @@
         <v>615</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>144</v>
@@ -4770,13 +4766,13 @@
         <v>625</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>184</v>
@@ -4814,13 +4810,13 @@
         <v>645</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>271</v>
@@ -4858,13 +4854,13 @@
         <v>590</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>45</v>
@@ -4902,13 +4898,13 @@
         <v>596</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>69</v>
@@ -4946,13 +4942,13 @@
         <v>601</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>89</v>
@@ -4990,13 +4986,13 @@
         <v>611</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>128</v>
@@ -5034,13 +5030,13 @@
         <v>616</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="N27" s="2" t="s">
         <v>148</v>
@@ -5078,13 +5074,13 @@
         <v>623</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>176</v>
@@ -5122,13 +5118,13 @@
         <v>630</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>208</v>
@@ -5166,13 +5162,13 @@
         <v>640</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>248</v>
@@ -5210,13 +5206,13 @@
         <v>641</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="N31" s="2" t="s">
         <v>252</v>
@@ -5254,13 +5250,13 @@
         <v>653</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="N32" s="2" t="s">
         <v>299</v>
@@ -5298,13 +5294,13 @@
         <v>654</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="N33" s="2" t="s">
         <v>303</v>
@@ -5342,13 +5338,13 @@
         <v>667</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>375</v>
@@ -5386,13 +5382,13 @@
         <v>586</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>29</v>
@@ -5430,13 +5426,13 @@
         <v>597</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>73</v>
@@ -5474,13 +5470,13 @@
         <v>612</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>132</v>
@@ -5518,13 +5514,13 @@
         <v>632</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>216</v>
@@ -5562,10 +5558,10 @@
         <v>646</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="M39"/>
       <c r="N39" s="2" t="s">
@@ -5576,7 +5572,7 @@
       <c r="A40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="6" t="s">
         <v>565</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -5588,7 +5584,7 @@
       <c r="E40" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="6" t="s">
         <v>522</v>
       </c>
       <c r="G40" s="2">
@@ -5600,17 +5596,17 @@
       <c r="I40" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J40" s="10" t="s">
+      <c r="J40" s="7" t="s">
         <v>583</v>
       </c>
-      <c r="K40" s="10" t="s">
-        <v>672</v>
-      </c>
-      <c r="L40" s="10" t="s">
-        <v>744</v>
-      </c>
-      <c r="M40" s="10" t="s">
-        <v>922</v>
+      <c r="K40" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="L40" s="7" t="s">
+        <v>742</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>920</v>
       </c>
       <c r="N40" s="2" t="s">
         <v>18</v>
@@ -5651,10 +5647,10 @@
         <v>668</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="N41" s="2" t="s">
         <v>4</v>
@@ -5695,10 +5691,10 @@
         <v>669</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="N42" s="2" t="s">
         <v>8</v>
@@ -5736,13 +5732,13 @@
         <v>587</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="N43" s="2" t="s">
         <v>33</v>
@@ -5780,13 +5776,13 @@
         <v>599</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="N44" s="2" t="s">
         <v>81</v>
@@ -5824,13 +5820,13 @@
         <v>600</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="N45" s="2" t="s">
         <v>85</v>
@@ -5868,13 +5864,13 @@
         <v>613</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="N46" s="2" t="s">
         <v>136</v>
@@ -5912,13 +5908,13 @@
         <v>624</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="N47" s="2" t="s">
         <v>180</v>
@@ -5956,13 +5952,13 @@
         <v>629</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="N48" s="2" t="s">
         <v>204</v>
@@ -6000,13 +5996,13 @@
         <v>634</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>224</v>
@@ -6044,13 +6040,13 @@
         <v>636</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="N50" s="2" t="s">
         <v>232</v>
@@ -6088,13 +6084,13 @@
         <v>637</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="N51" s="2" t="s">
         <v>236</v>
@@ -6132,13 +6128,13 @@
         <v>643</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>259</v>
@@ -6176,13 +6172,13 @@
         <v>643</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="N53" s="2" t="s">
         <v>263</v>
@@ -6220,13 +6216,13 @@
         <v>644</v>
       </c>
       <c r="K54" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="N54" s="2" t="s">
         <v>267</v>
@@ -6264,13 +6260,13 @@
         <v>647</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="N55" s="2" t="s">
         <v>275</v>
@@ -6308,13 +6304,13 @@
         <v>651</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>291</v>
@@ -6352,13 +6348,13 @@
         <v>662</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="N57" s="2" t="s">
         <v>351</v>
@@ -6396,13 +6392,13 @@
         <v>662</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="N58" s="2" t="s">
         <v>355</v>
@@ -6440,13 +6436,13 @@
         <v>588</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>37</v>
@@ -6484,13 +6480,13 @@
         <v>592</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="N60" s="2" t="s">
         <v>53</v>
@@ -6528,13 +6524,13 @@
         <v>595</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="N61" s="2" t="s">
         <v>65</v>
@@ -6572,13 +6568,13 @@
         <v>598</v>
       </c>
       <c r="K62" s="3" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="N62" s="2" t="s">
         <v>77</v>
@@ -6616,13 +6612,13 @@
         <v>605</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="N63" s="2" t="s">
         <v>104</v>
@@ -6660,13 +6656,13 @@
         <v>614</v>
       </c>
       <c r="K64" s="3" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="N64" s="2" t="s">
         <v>140</v>
@@ -6704,13 +6700,13 @@
         <v>617</v>
       </c>
       <c r="K65" s="3" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="N65" s="2" t="s">
         <v>152</v>
@@ -6748,13 +6744,13 @@
         <v>622</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="N66" s="2" t="s">
         <v>172</v>
@@ -6792,13 +6788,13 @@
         <v>626</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="N67" s="2" t="s">
         <v>192</v>
@@ -6836,13 +6832,13 @@
         <v>628</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="M68" s="3" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="N68" s="2" t="s">
         <v>200</v>
@@ -6880,13 +6876,13 @@
         <v>631</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="L69" s="3" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="M69" s="3" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="N69" s="2" t="s">
         <v>212</v>
@@ -6924,13 +6920,13 @@
         <v>635</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="L70" s="3" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="M70" s="3" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="N70" s="2" t="s">
         <v>228</v>
@@ -6968,13 +6964,13 @@
         <v>638</v>
       </c>
       <c r="K71" s="3" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="M71" s="3" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="N71" s="2" t="s">
         <v>240</v>
@@ -7012,13 +7008,13 @@
         <v>650</v>
       </c>
       <c r="K72" s="3" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="M72" s="3" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="N72" s="2" t="s">
         <v>295</v>
@@ -7056,13 +7052,13 @@
         <v>660</v>
       </c>
       <c r="K73" s="3" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="M73" s="3" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="N73" s="2" t="s">
         <v>339</v>
@@ -7100,13 +7096,13 @@
         <v>660</v>
       </c>
       <c r="K74" s="3" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="N74" s="2" t="s">
         <v>343</v>
@@ -7144,13 +7140,13 @@
         <v>593</v>
       </c>
       <c r="K75" s="3" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="N75" s="2" t="s">
         <v>57</v>
@@ -7188,13 +7184,13 @@
         <v>659</v>
       </c>
       <c r="K76" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L76" s="3" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="N76" s="1" t="s">
         <v>335</v>
@@ -7232,13 +7228,13 @@
         <v>594</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="L77" s="3" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="N77" s="2" t="s">
         <v>61</v>
@@ -7276,13 +7272,13 @@
         <v>591</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="L78" s="3" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="M78" s="3" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="N78" s="1" t="s">
         <v>49</v>
@@ -7320,13 +7316,13 @@
         <v>620</v>
       </c>
       <c r="K79" s="3" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="L79" s="3" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M79" s="3" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="N79" s="1" t="s">
         <v>164</v>
@@ -7364,13 +7360,13 @@
         <v>639</v>
       </c>
       <c r="K80" s="3" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="L80" s="3" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="M80" s="3" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="N80" s="1" t="s">
         <v>244</v>
@@ -7408,13 +7404,13 @@
         <v>663</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="L81" s="3" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="M81" s="3" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="N81" s="1" t="s">
         <v>359</v>
@@ -7452,13 +7448,13 @@
         <v>606</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="L82" s="3" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="M82" s="3" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="N82" s="1" t="s">
         <v>108</v>
@@ -7496,13 +7492,13 @@
         <v>619</v>
       </c>
       <c r="K83" s="3" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="L83" s="3" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="M83" s="3" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="N83" s="1" t="s">
         <v>160</v>
@@ -7540,13 +7536,13 @@
         <v>652</v>
       </c>
       <c r="K84" s="3" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="L84" s="3" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="M84" s="3" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="N84" s="1" t="s">
         <v>307</v>
@@ -7584,13 +7580,13 @@
         <v>602</v>
       </c>
       <c r="K85" s="3" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="M85" s="3" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="N85" s="1" t="s">
         <v>93</v>
@@ -7628,13 +7624,13 @@
         <v>648</v>
       </c>
       <c r="K86" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="M86" s="3" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="N86" s="1" t="s">
         <v>279</v>
@@ -7672,13 +7668,13 @@
         <v>648</v>
       </c>
       <c r="K87" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="L87" s="3" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="M87" s="3" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="N87" s="1" t="s">
         <v>283</v>
@@ -7714,10 +7710,10 @@
       </c>
       <c r="K88"/>
       <c r="L88" s="3" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="M88" s="3" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="N88" s="1" t="s">
         <v>188</v>
@@ -7755,13 +7751,13 @@
         <v>627</v>
       </c>
       <c r="K89" s="3" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="L89" s="3" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="M89" s="3" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="N89" s="1" t="s">
         <v>196</v>
@@ -7799,13 +7795,13 @@
         <v>655</v>
       </c>
       <c r="K90" s="3" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="L90" s="3" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="M90" s="3" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="N90" s="1" t="s">
         <v>315</v>
@@ -7843,13 +7839,13 @@
         <v>607</v>
       </c>
       <c r="K91" s="3" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="L91" s="3" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="M91" s="3" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="N91" s="1" t="s">
         <v>112</v>
@@ -7887,13 +7883,13 @@
         <v>608</v>
       </c>
       <c r="K92" s="3" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="L92" s="3" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="M92" s="3" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="N92" s="1" t="s">
         <v>116</v>
@@ -7931,13 +7927,13 @@
         <v>621</v>
       </c>
       <c r="K93" s="3" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="L93" s="3" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="M93" s="3" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="N93" s="1" t="s">
         <v>168</v>
@@ -7975,13 +7971,13 @@
         <v>657</v>
       </c>
       <c r="K94" s="3" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="L94" s="3" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="M94" s="3" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="N94" s="1" t="s">
         <v>327</v>
@@ -8019,13 +8015,13 @@
         <v>585</v>
       </c>
       <c r="K95" s="3" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="L95" s="3" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="M95" s="3" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="N95" s="1" t="s">
         <v>25</v>
@@ -8063,13 +8059,13 @@
         <v>664</v>
       </c>
       <c r="K96" s="3" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="L96" s="3" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="M96" s="3" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="N96" s="1" t="s">
         <v>363</v>
@@ -8104,16 +8100,16 @@
         <v>378</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="L97" s="3" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="M97" s="3" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="N97" s="1" t="s">
         <v>379</v>
@@ -8148,16 +8144,16 @@
         <v>382</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="K98" s="3" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="L98" s="3" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="M98" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="N98" s="1" t="s">
         <v>383</v>

</xml_diff>